<commit_message>
added unit tests for checking correct integers and dates
</commit_message>
<xml_diff>
--- a/src/test/resources/School_Student_Information.xlsx
+++ b/src/test/resources/School_Student_Information.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,7 +499,7 @@
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -548,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -579,6 +579,9 @@
       </c>
       <c r="L2">
         <v>3312343235</v>
+      </c>
+      <c r="M2" s="2">
+        <v>38635</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -618,6 +621,9 @@
       <c r="L3">
         <v>3509238462</v>
       </c>
+      <c r="M3" s="2">
+        <v>38635</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -656,6 +662,9 @@
       <c r="L4">
         <v>3310943274</v>
       </c>
+      <c r="M4" s="2">
+        <v>38635</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -693,6 +702,9 @@
       </c>
       <c r="L5">
         <v>3452424435</v>
+      </c>
+      <c r="M5" s="2">
+        <v>38635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new class for cell parsing and added a suite for parser related unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/School_Student_Information.xlsx
+++ b/src/test/resources/School_Student_Information.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Registration#</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Mother's Name</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -196,10 +202,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -479,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,9 +507,11 @@
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,8 +551,14 @@
       <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -583,8 +598,14 @@
       <c r="M2" s="2">
         <v>38635</v>
       </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>23.41</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -624,8 +645,14 @@
       <c r="M3" s="2">
         <v>38635</v>
       </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>21.67</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -665,8 +692,14 @@
       <c r="M4" s="2">
         <v>38635</v>
       </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>29.32</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -705,6 +738,12 @@
       </c>
       <c r="M5" s="2">
         <v>38635</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>22.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed code+unit tests for cell deserializer
</commit_message>
<xml_diff>
--- a/src/test/resources/School_Student_Information.xlsx
+++ b/src/test/resources/School_Student_Information.xlsx
@@ -107,9 +107,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Girl</t>
-  </si>
-  <si>
     <t>Bing</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -197,8 +197,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -208,9 +210,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,7 +493,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -549,13 +553,13 @@
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -634,7 +638,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2">
         <v>38620</v>
@@ -672,16 +676,16 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="2">
         <v>38601</v>
@@ -716,19 +720,19 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
         <v>23</v>
       </c>
       <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
       </c>
       <c r="K5" s="2">
         <v>38401</v>

</xml_diff>